<commit_message>
a little change to the database
</commit_message>
<xml_diff>
--- a/database_scheme.xlsx
+++ b/database_scheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="-520" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,10 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>playlist id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>download time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>keywords</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -278,19 +270,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>comment?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>favorite list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>channel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>subscribe channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>media_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>media_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gender</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -454,7 +474,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="112">
+  <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -567,8 +587,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="43"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -591,13 +613,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="43" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="43" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="43" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="43" applyBorder="1" applyAlignment="1">
@@ -612,14 +630,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="112">
+  <cellStyles count="114">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -675,6 +696,7 @@
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -730,6 +752,7 @@
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="43" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1060,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1072,21 +1095,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="N1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="17"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="N1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
@@ -1101,18 +1124,20 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="I2" s="16"/>
+      <c r="E2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="15"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1120,9 +1145,9 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="I3" s="16"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="N3" s="1"/>
@@ -1133,9 +1158,9 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="I4" s="16"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="N4" s="1"/>
@@ -1146,9 +1171,9 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="I5" s="16"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="N5" s="1"/>
@@ -1157,32 +1182,32 @@
     <row r="6" spans="1:16">
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="G7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="G7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="20"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:16">
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1198,81 +1223,81 @@
       <c r="H10" s="1"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="H12" s="20" t="s">
+      <c r="A12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="M12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
+      <c r="I12" s="18"/>
+      <c r="M12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="H13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="18"/>
+      <c r="P13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="H13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="20"/>
-      <c r="P13" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="3"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
       <c r="H14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N14" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="O14" s="20"/>
+      <c r="N14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="18"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="18"/>
       <c r="H15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="7"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16">
@@ -1280,77 +1305,82 @@
       <c r="B16" s="2"/>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="20" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="20"/>
+      <c r="E19" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
       <c r="J19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="5"/>
-      <c r="N19" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
+      <c r="N19" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="20">
+      <c r="A20" s="18">
         <v>1</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="1">
         <v>2</v>
       </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="N20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="20">
+      <c r="A21" s="18">
         <v>1</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="1">
         <v>3</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1368,18 +1398,21 @@
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>11</v>
@@ -1389,11 +1422,12 @@
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
         <v>5</v>
@@ -1402,104 +1436,98 @@
         <v>5</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="22"/>
+      <c r="A27" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="20"/>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="20"/>
+      <c r="G28" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="21" t="s">
+      <c r="H28" s="20"/>
+      <c r="I28" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="10" t="s">
+      <c r="J28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="21" t="s">
+      <c r="M28" s="20"/>
+      <c r="N28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M28" s="22"/>
-      <c r="N28" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O28" s="15" t="s">
+      <c r="O28" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="P28" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q28" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="R28" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="S28" s="11" t="s">
-        <v>68</v>
-      </c>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="11"/>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="1">
         <v>3</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10">
         <v>4</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="19">
         <v>4</v>
       </c>
-      <c r="K29" s="22"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="3"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="20"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
@@ -1509,41 +1537,51 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B32" s="13"/>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="O32" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P32" s="17"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
       <c r="M33" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="O33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>6</v>
@@ -1552,62 +1590,110 @@
       <c r="I34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="17" t="s">
+      <c r="J34" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="19"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="17"/>
       <c r="M34" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="E36" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="E37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="M12:P12"/>
+  <mergeCells count="38">
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="A27:S27"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:H28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N13:O13"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>